<commit_message>
final changes and results
</commit_message>
<xml_diff>
--- a/igvz/data/data_scores.xlsx
+++ b/igvz/data/data_scores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10424"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nextgenmetrics-my.sharepoint.com/personal/nagesh_nextgenmetrics_com/Documents/Personal/Anisha/M3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_05FA832D5656A12AD83CBF4E315EE561A1A9F47B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0892C7EB-B39F-944D-B01C-2704B53F4404}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="11_05FA832D5656A12AD83CBF4E315EE561A1A9F47B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4379C43-3F69-3C43-A745-AE7BB7D388E4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'v.10 IGVZ database 4 + controle'!$A$1:$AZ$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -623,6 +636,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -912,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -925,7 +942,24 @@
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="3"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="32.1640625" customWidth="1"/>
+    <col min="12" max="12" width="27.6640625" customWidth="1"/>
+    <col min="13" max="13" width="33.33203125" customWidth="1"/>
+    <col min="14" max="14" width="29.6640625" customWidth="1"/>
+    <col min="15" max="15" width="22.6640625" customWidth="1"/>
+    <col min="16" max="16" width="36.6640625" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.5" customWidth="1"/>
+    <col min="19" max="19" width="26.1640625" customWidth="1"/>
+    <col min="20" max="20" width="24" customWidth="1"/>
+    <col min="21" max="21" width="22.83203125" customWidth="1"/>
+    <col min="22" max="22" width="20.1640625" customWidth="1"/>
+    <col min="23" max="23" width="18.5" customWidth="1"/>
+    <col min="24" max="24" width="20.1640625" customWidth="1"/>
+    <col min="25" max="25" width="19.33203125" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" customWidth="1"/>
+    <col min="27" max="27" width="17.5" customWidth="1"/>
     <col min="28" max="28" width="20.33203125" customWidth="1"/>
     <col min="29" max="29" width="15.83203125" customWidth="1"/>
     <col min="30" max="30" width="20.6640625" customWidth="1"/>
@@ -1187,7 +1221,8 @@
         <v>0</v>
       </c>
       <c r="AD2" s="3">
-        <v>10</v>
+        <f>SUM(I2:AC2)</f>
+        <v>11</v>
       </c>
       <c r="AE2" s="3">
         <v>0</v>
@@ -1345,7 +1380,8 @@
         <v>1</v>
       </c>
       <c r="AD3" s="3">
-        <v>11</v>
+        <f t="shared" ref="AD3:AD66" si="0">SUM(I3:AC3)</f>
+        <v>12</v>
       </c>
       <c r="AE3" s="3">
         <v>1</v>
@@ -1503,7 +1539,8 @@
         <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="AE4" s="3">
         <v>0</v>
@@ -1661,7 +1698,8 @@
         <v>1</v>
       </c>
       <c r="AD5" s="3">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="AE5" s="3">
         <v>0</v>
@@ -1819,7 +1857,8 @@
         <v>0</v>
       </c>
       <c r="AD6" s="3">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="AE6" s="3">
         <v>0</v>
@@ -1977,7 +2016,8 @@
         <v>1</v>
       </c>
       <c r="AD7" s="3">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="AE7" s="3">
         <v>0</v>
@@ -2135,7 +2175,8 @@
         <v>1</v>
       </c>
       <c r="AD8" s="3">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="AE8" s="3">
         <v>0</v>
@@ -2293,6 +2334,7 @@
         <v>1</v>
       </c>
       <c r="AD9" s="3">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="AE9" s="3">
@@ -2451,7 +2493,8 @@
         <v>0</v>
       </c>
       <c r="AD10" s="3">
-        <v>99</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="AE10" s="3">
         <v>0</v>
@@ -2609,7 +2652,8 @@
         <v>0</v>
       </c>
       <c r="AD11" s="3">
-        <v>99</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="AE11" s="3">
         <v>0</v>
@@ -2767,6 +2811,7 @@
         <v>1</v>
       </c>
       <c r="AD12" s="3">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="AE12" s="3">
@@ -2925,6 +2970,7 @@
         <v>1</v>
       </c>
       <c r="AD13" s="3">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="AE13" s="3">
@@ -3083,6 +3129,7 @@
         <v>1</v>
       </c>
       <c r="AD14" s="3">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="AE14" s="3">
@@ -3241,6 +3288,7 @@
         <v>1</v>
       </c>
       <c r="AD15" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="AE15" s="3">
@@ -3399,7 +3447,8 @@
         <v>1</v>
       </c>
       <c r="AD16" s="3">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="AE16" s="3">
         <v>0</v>
@@ -3557,7 +3606,8 @@
         <v>1</v>
       </c>
       <c r="AD17" s="3">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="AE17" s="3">
         <v>1</v>
@@ -3715,7 +3765,8 @@
         <v>0</v>
       </c>
       <c r="AD18" s="3">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="AE18" s="3">
         <v>0</v>
@@ -3873,7 +3924,8 @@
         <v>1</v>
       </c>
       <c r="AD19" s="3">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="AE19" s="3">
         <v>1</v>
@@ -4031,7 +4083,8 @@
         <v>0</v>
       </c>
       <c r="AD20" s="3">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="AE20" s="3">
         <v>1</v>
@@ -4189,6 +4242,7 @@
         <v>1</v>
       </c>
       <c r="AD21" s="3">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="AE21" s="3">
@@ -4347,6 +4401,7 @@
         <v>1</v>
       </c>
       <c r="AD22" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="AE22" s="3">
@@ -4505,6 +4560,7 @@
         <v>1</v>
       </c>
       <c r="AD23" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AE23" s="3">
@@ -4663,6 +4719,7 @@
         <v>1</v>
       </c>
       <c r="AD24" s="3">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AE24" s="3">
@@ -4821,6 +4878,7 @@
         <v>1</v>
       </c>
       <c r="AD25" s="3">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="AE25" s="3">
@@ -4979,7 +5037,8 @@
         <v>1</v>
       </c>
       <c r="AD26" s="3">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="AE26" s="3">
         <v>0</v>
@@ -5137,7 +5196,8 @@
         <v>1</v>
       </c>
       <c r="AD27" s="3">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="AE27" s="3">
         <v>1</v>
@@ -5295,7 +5355,8 @@
         <v>1</v>
       </c>
       <c r="AD28" s="3">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="AE28" s="3">
         <v>1</v>
@@ -5453,7 +5514,8 @@
         <v>1</v>
       </c>
       <c r="AD29" s="3">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="AE29" s="3">
         <v>1</v>
@@ -5611,6 +5673,7 @@
         <v>0</v>
       </c>
       <c r="AD30" s="3">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AE30" s="3">
@@ -5769,7 +5832,8 @@
         <v>0</v>
       </c>
       <c r="AD31" s="3">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="AE31" s="3">
         <v>1</v>
@@ -5927,7 +5991,8 @@
         <v>0</v>
       </c>
       <c r="AD32" s="3">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="AE32" s="3">
         <v>0</v>
@@ -6085,7 +6150,8 @@
         <v>1</v>
       </c>
       <c r="AD33" s="3">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="AE33" s="3">
         <v>0</v>
@@ -6243,6 +6309,7 @@
         <v>0</v>
       </c>
       <c r="AD34" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AE34" s="3">
@@ -6401,7 +6468,8 @@
         <v>0</v>
       </c>
       <c r="AD35" s="3">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="AE35" s="3">
         <v>1</v>
@@ -6559,6 +6627,7 @@
         <v>0</v>
       </c>
       <c r="AD36" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE36" s="3">
@@ -6717,6 +6786,7 @@
         <v>0</v>
       </c>
       <c r="AD37" s="3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="AE37" s="3">
@@ -6875,7 +6945,8 @@
         <v>1</v>
       </c>
       <c r="AD38" s="3">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="AE38" s="3">
         <v>0</v>
@@ -7033,6 +7104,7 @@
         <v>1</v>
       </c>
       <c r="AD39" s="3">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="AE39" s="3">
@@ -7191,6 +7263,7 @@
         <v>0</v>
       </c>
       <c r="AD40" s="3">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AE40" s="3">
@@ -7349,6 +7422,7 @@
         <v>0</v>
       </c>
       <c r="AD41" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="AE41" s="3">
@@ -7507,7 +7581,8 @@
         <v>0</v>
       </c>
       <c r="AD42" s="3">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="AE42" s="3">
         <v>1</v>
@@ -7665,6 +7740,7 @@
         <v>1</v>
       </c>
       <c r="AD43" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AE43" s="3">
@@ -7823,6 +7899,7 @@
         <v>1</v>
       </c>
       <c r="AD44" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AE44" s="3">
@@ -7981,6 +8058,7 @@
         <v>1</v>
       </c>
       <c r="AD45" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AE45" s="3">
@@ -8139,6 +8217,7 @@
         <v>1</v>
       </c>
       <c r="AD46" s="3">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="AE46" s="3">
@@ -8297,7 +8376,8 @@
         <v>0</v>
       </c>
       <c r="AD47" s="3">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="AE47" s="3">
         <v>0</v>
@@ -8455,7 +8535,8 @@
         <v>1</v>
       </c>
       <c r="AD48" s="3">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="AE48" s="3">
         <v>1</v>
@@ -8613,7 +8694,8 @@
         <v>1</v>
       </c>
       <c r="AD49" s="3">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="AE49" s="3">
         <v>0</v>
@@ -8771,7 +8853,8 @@
         <v>1</v>
       </c>
       <c r="AD50" s="3">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="AE50" s="3">
         <v>0</v>
@@ -8929,6 +9012,7 @@
         <v>0</v>
       </c>
       <c r="AD51" s="3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="AE51" s="3">
@@ -9087,7 +9171,8 @@
         <v>1</v>
       </c>
       <c r="AD52" s="3">
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="AE52" s="3">
         <v>1</v>
@@ -9245,6 +9330,7 @@
         <v>1</v>
       </c>
       <c r="AD53" s="3">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="AE53" s="3">
@@ -9403,7 +9489,8 @@
         <v>0</v>
       </c>
       <c r="AD54" s="3">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="AE54" s="3">
         <v>0</v>
@@ -9561,6 +9648,7 @@
         <v>1</v>
       </c>
       <c r="AD55" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AE55" s="3">
@@ -9719,7 +9807,8 @@
         <v>1</v>
       </c>
       <c r="AD56" s="3">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="AE56" s="3">
         <v>0</v>
@@ -9877,6 +9966,7 @@
         <v>1</v>
       </c>
       <c r="AD57" s="3">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="AE57" s="3">
@@ -10035,6 +10125,7 @@
         <v>1</v>
       </c>
       <c r="AD58" s="3">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="AE58" s="3">
@@ -10193,6 +10284,7 @@
         <v>1</v>
       </c>
       <c r="AD59" s="3">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="AE59" s="3">
@@ -10351,6 +10443,7 @@
         <v>0</v>
       </c>
       <c r="AD60" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE60" s="3">
@@ -10509,7 +10602,8 @@
         <v>1</v>
       </c>
       <c r="AD61" s="3">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="AE61" s="3">
         <v>1</v>
@@ -10667,6 +10761,7 @@
         <v>1</v>
       </c>
       <c r="AD62" s="3">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="AE62" s="3">
@@ -10825,6 +10920,7 @@
         <v>1</v>
       </c>
       <c r="AD63" s="3">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="AE63" s="3">
@@ -10983,6 +11079,7 @@
         <v>1</v>
       </c>
       <c r="AD64" s="3">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="AE64" s="3">
@@ -11141,6 +11238,7 @@
         <v>0</v>
       </c>
       <c r="AD65" s="3">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="AE65" s="3">
@@ -11299,6 +11397,7 @@
         <v>1</v>
       </c>
       <c r="AD66" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="AE66" s="3">
@@ -11457,7 +11556,8 @@
         <v>0</v>
       </c>
       <c r="AD67" s="3">
-        <v>7</v>
+        <f t="shared" ref="AD67:AD130" si="1">SUM(I67:AC67)</f>
+        <v>8</v>
       </c>
       <c r="AE67" s="3">
         <v>0</v>
@@ -11615,7 +11715,8 @@
         <v>1</v>
       </c>
       <c r="AD68" s="3">
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="AE68" s="3">
         <v>0</v>
@@ -11773,7 +11874,8 @@
         <v>1</v>
       </c>
       <c r="AD69" s="3">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="AE69" s="3">
         <v>0</v>
@@ -11931,6 +12033,7 @@
         <v>1</v>
       </c>
       <c r="AD70" s="3">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="AE70" s="3">
@@ -12089,6 +12192,7 @@
         <v>0</v>
       </c>
       <c r="AD71" s="3">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE71" s="3">
@@ -12247,7 +12351,8 @@
         <v>1</v>
       </c>
       <c r="AD72" s="3">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="AE72" s="3">
         <v>0</v>
@@ -12405,7 +12510,8 @@
         <v>1</v>
       </c>
       <c r="AD73" s="3">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="AE73" s="3">
         <v>0</v>
@@ -12563,7 +12669,8 @@
         <v>1</v>
       </c>
       <c r="AD74" s="3">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="AE74" s="3">
         <v>0</v>
@@ -12721,7 +12828,8 @@
         <v>1</v>
       </c>
       <c r="AD75" s="3">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="AE75" s="3">
         <v>0</v>
@@ -12879,6 +12987,7 @@
         <v>0</v>
       </c>
       <c r="AD76" s="3">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE76" s="3">
@@ -13037,7 +13146,8 @@
         <v>1</v>
       </c>
       <c r="AD77" s="3">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="AE77" s="3">
         <v>1</v>
@@ -13195,7 +13305,8 @@
         <v>0</v>
       </c>
       <c r="AD78" s="3">
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="AE78" s="3">
         <v>1</v>
@@ -13353,7 +13464,8 @@
         <v>0</v>
       </c>
       <c r="AD79" s="3">
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="AE79" s="3">
         <v>0</v>
@@ -13511,7 +13623,8 @@
         <v>0</v>
       </c>
       <c r="AD80" s="3">
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="AE80" s="3">
         <v>0</v>
@@ -13669,6 +13782,7 @@
         <v>1</v>
       </c>
       <c r="AD81" s="3">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="AE81" s="3">
@@ -13827,7 +13941,8 @@
         <v>0</v>
       </c>
       <c r="AD82" s="3">
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="AE82" s="3">
         <v>0</v>
@@ -13985,6 +14100,7 @@
         <v>0</v>
       </c>
       <c r="AD83" s="3">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AE83" s="3">
@@ -14143,7 +14259,8 @@
         <v>1</v>
       </c>
       <c r="AD84" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="AE84" s="3">
         <v>1</v>
@@ -14301,7 +14418,8 @@
         <v>0</v>
       </c>
       <c r="AD85" s="3">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="AE85" s="3">
         <v>0</v>
@@ -14459,7 +14577,8 @@
         <v>0</v>
       </c>
       <c r="AD86" s="3">
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="AE86" s="3">
         <v>0</v>
@@ -14617,7 +14736,8 @@
         <v>0</v>
       </c>
       <c r="AD87" s="3">
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="AE87" s="3">
         <v>0</v>
@@ -14775,7 +14895,8 @@
         <v>0</v>
       </c>
       <c r="AD88" s="3">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AE88" s="3">
         <v>1</v>
@@ -14933,6 +15054,7 @@
         <v>1</v>
       </c>
       <c r="AD89" s="3">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="AE89" s="3">
@@ -15091,7 +15213,8 @@
         <v>1</v>
       </c>
       <c r="AD90" s="3">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="AE90" s="3">
         <v>1</v>
@@ -15249,7 +15372,8 @@
         <v>1</v>
       </c>
       <c r="AD91" s="3">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="AE91" s="3">
         <v>1</v>
@@ -15407,7 +15531,8 @@
         <v>0</v>
       </c>
       <c r="AD92" s="3">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="AE92" s="3">
         <v>1</v>
@@ -15565,7 +15690,8 @@
         <v>1</v>
       </c>
       <c r="AD93" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="AE93" s="3">
         <v>0</v>
@@ -15723,7 +15849,8 @@
         <v>1</v>
       </c>
       <c r="AD94" s="3">
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="AE94" s="3">
         <v>1</v>
@@ -15881,6 +16008,7 @@
         <v>1</v>
       </c>
       <c r="AD95" s="3">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AE95" s="3">
@@ -16039,7 +16167,8 @@
         <v>1</v>
       </c>
       <c r="AD96" s="3">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="AE96" s="3">
         <v>1</v>
@@ -16197,7 +16326,8 @@
         <v>1</v>
       </c>
       <c r="AD97" s="3">
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="AE97" s="3">
         <v>0</v>
@@ -16355,6 +16485,7 @@
         <v>1</v>
       </c>
       <c r="AD98" s="3">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AE98" s="3">
@@ -16513,7 +16644,8 @@
         <v>1</v>
       </c>
       <c r="AD99" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="AE99" s="3">
         <v>1</v>
@@ -16671,7 +16803,8 @@
         <v>1</v>
       </c>
       <c r="AD100" s="3">
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="AE100" s="3">
         <v>0</v>
@@ -16829,7 +16962,8 @@
         <v>1</v>
       </c>
       <c r="AD101" s="3">
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="AE101" s="3">
         <v>0</v>
@@ -16987,7 +17121,8 @@
         <v>0</v>
       </c>
       <c r="AD102" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="AE102" s="3">
         <v>1</v>
@@ -17145,7 +17280,8 @@
         <v>1</v>
       </c>
       <c r="AD103" s="3">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="AE103" s="3">
         <v>0</v>
@@ -17303,7 +17439,8 @@
         <v>1</v>
       </c>
       <c r="AD104" s="3">
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="AE104" s="3">
         <v>0</v>
@@ -17461,7 +17598,8 @@
         <v>0</v>
       </c>
       <c r="AD105" s="3">
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="AE105" s="3">
         <v>1</v>
@@ -17619,7 +17757,8 @@
         <v>1</v>
       </c>
       <c r="AD106" s="3">
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="AE106" s="3">
         <v>0</v>
@@ -17777,7 +17916,8 @@
         <v>1</v>
       </c>
       <c r="AD107" s="3">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="AE107" s="3">
         <v>1</v>
@@ -17935,6 +18075,7 @@
         <v>1</v>
       </c>
       <c r="AD108" s="3">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="AE108" s="3">
@@ -18093,6 +18234,7 @@
         <v>1</v>
       </c>
       <c r="AD109" s="3">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="AE109" s="3">
@@ -18251,6 +18393,7 @@
         <v>1</v>
       </c>
       <c r="AD110" s="3">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="AE110" s="3">
@@ -18409,6 +18552,7 @@
         <v>0</v>
       </c>
       <c r="AD111" s="3">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="AE111" s="3">
@@ -18567,7 +18711,8 @@
         <v>1</v>
       </c>
       <c r="AD112" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="AE112" s="3">
         <v>0</v>
@@ -18725,6 +18870,7 @@
         <v>0</v>
       </c>
       <c r="AD113" s="3">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="AE113" s="3">
@@ -18883,7 +19029,8 @@
         <v>1</v>
       </c>
       <c r="AD114" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="AE114" s="3">
         <v>0</v>
@@ -19041,7 +19188,8 @@
         <v>1</v>
       </c>
       <c r="AD115" s="3">
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="AE115" s="3">
         <v>0</v>
@@ -19199,6 +19347,7 @@
         <v>1</v>
       </c>
       <c r="AD116" s="3">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AE116" s="3">
@@ -19357,7 +19506,8 @@
         <v>1</v>
       </c>
       <c r="AD117" s="3">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="AE117" s="3">
         <v>0</v>
@@ -19515,6 +19665,7 @@
         <v>1</v>
       </c>
       <c r="AD118" s="3">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="AE118" s="3">
@@ -19673,6 +19824,7 @@
         <v>0</v>
       </c>
       <c r="AD119" s="3">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="AE119" s="3">
@@ -19831,6 +19983,7 @@
         <v>1</v>
       </c>
       <c r="AD120" s="3">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AE120" s="3">
@@ -19989,6 +20142,7 @@
         <v>1</v>
       </c>
       <c r="AD121" s="3">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="AE121" s="3">
@@ -20147,7 +20301,8 @@
         <v>1</v>
       </c>
       <c r="AD122" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="AE122" s="3">
         <v>0</v>
@@ -20305,6 +20460,7 @@
         <v>1</v>
       </c>
       <c r="AD123" s="3">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="AE123" s="3">
@@ -20463,7 +20619,8 @@
         <v>1</v>
       </c>
       <c r="AD124" s="3">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="AE124" s="3">
         <v>1</v>
@@ -20621,6 +20778,7 @@
         <v>1</v>
       </c>
       <c r="AD125" s="3">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AE125" s="3">
@@ -20779,7 +20937,8 @@
         <v>0</v>
       </c>
       <c r="AD126" s="3">
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="AE126" s="3">
         <v>0</v>
@@ -20937,6 +21096,7 @@
         <v>1</v>
       </c>
       <c r="AD127" s="3">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AE127" s="3">
@@ -21095,7 +21255,8 @@
         <v>1</v>
       </c>
       <c r="AD128" s="3">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="AE128" s="3">
         <v>1</v>
@@ -21253,7 +21414,8 @@
         <v>1</v>
       </c>
       <c r="AD129" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="AE129" s="3">
         <v>1</v>
@@ -21411,7 +21573,8 @@
         <v>1</v>
       </c>
       <c r="AD130" s="3">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="AE130" s="3">
         <v>0</v>
@@ -21569,7 +21732,8 @@
         <v>1</v>
       </c>
       <c r="AD131" s="3">
-        <v>4</v>
+        <f t="shared" ref="AD131" si="2">SUM(I131:AC131)</f>
+        <v>5</v>
       </c>
       <c r="AE131" s="3">
         <v>0</v>

</xml_diff>